<commit_message>
upload game sim results(350) from azure VM
</commit_message>
<xml_diff>
--- a/7WondersGameResultsAzure.xlsx
+++ b/7WondersGameResultsAzure.xlsx
@@ -3872,7 +3872,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:L349"/>
+  <dimension ref="A1:L451"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -15046,6 +15046,3270 @@
         <v>2</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" s="0">
+        <v>41</v>
+      </c>
+      <c r="B350" s="0">
+        <v>48</v>
+      </c>
+      <c r="C350" s="0">
+        <v>59</v>
+      </c>
+      <c r="D350" s="0">
+        <v>42</v>
+      </c>
+      <c r="E350" s="0">
+        <v>38</v>
+      </c>
+      <c r="H350" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I350" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J350" s="0">
+        <v>2</v>
+      </c>
+      <c r="K350" s="0">
+        <v>59</v>
+      </c>
+      <c r="L350" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" s="0">
+        <v>49</v>
+      </c>
+      <c r="B351" s="0">
+        <v>55</v>
+      </c>
+      <c r="C351" s="0">
+        <v>42</v>
+      </c>
+      <c r="D351" s="0">
+        <v>45</v>
+      </c>
+      <c r="E351" s="0">
+        <v>33</v>
+      </c>
+      <c r="H351" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I351" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="J351" s="0">
+        <v>1</v>
+      </c>
+      <c r="K351" s="0">
+        <v>55</v>
+      </c>
+      <c r="L351" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="0">
+        <v>64</v>
+      </c>
+      <c r="B352" s="0">
+        <v>38</v>
+      </c>
+      <c r="C352" s="0">
+        <v>46</v>
+      </c>
+      <c r="D352" s="0">
+        <v>63</v>
+      </c>
+      <c r="E352" s="0">
+        <v>29</v>
+      </c>
+      <c r="H352" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I352" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J352" s="0">
+        <v>0</v>
+      </c>
+      <c r="K352" s="0">
+        <v>64</v>
+      </c>
+      <c r="L352" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="0">
+        <v>58</v>
+      </c>
+      <c r="B353" s="0">
+        <v>36</v>
+      </c>
+      <c r="C353" s="0">
+        <v>48</v>
+      </c>
+      <c r="D353" s="0">
+        <v>42</v>
+      </c>
+      <c r="E353" s="0">
+        <v>52</v>
+      </c>
+      <c r="H353" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I353" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="J353" s="0">
+        <v>0</v>
+      </c>
+      <c r="K353" s="0">
+        <v>58</v>
+      </c>
+      <c r="L353" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="0">
+        <v>47</v>
+      </c>
+      <c r="B354" s="0">
+        <v>64</v>
+      </c>
+      <c r="C354" s="0">
+        <v>44</v>
+      </c>
+      <c r="D354" s="0">
+        <v>47</v>
+      </c>
+      <c r="E354" s="0">
+        <v>45</v>
+      </c>
+      <c r="H354" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="I354" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J354" s="0">
+        <v>1</v>
+      </c>
+      <c r="K354" s="0">
+        <v>64</v>
+      </c>
+      <c r="L354" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="0">
+        <v>43</v>
+      </c>
+      <c r="B355" s="0">
+        <v>44</v>
+      </c>
+      <c r="C355" s="0">
+        <v>56</v>
+      </c>
+      <c r="D355" s="0">
+        <v>44</v>
+      </c>
+      <c r="E355" s="0">
+        <v>41</v>
+      </c>
+      <c r="H355" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I355" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J355" s="0">
+        <v>2</v>
+      </c>
+      <c r="K355" s="0">
+        <v>56</v>
+      </c>
+      <c r="L355" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="0">
+        <v>44</v>
+      </c>
+      <c r="B356" s="0">
+        <v>40</v>
+      </c>
+      <c r="C356" s="0">
+        <v>53</v>
+      </c>
+      <c r="D356" s="0">
+        <v>59</v>
+      </c>
+      <c r="E356" s="0">
+        <v>35</v>
+      </c>
+      <c r="H356" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I356" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J356" s="0">
+        <v>3</v>
+      </c>
+      <c r="K356" s="0">
+        <v>59</v>
+      </c>
+      <c r="L356" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="0">
+        <v>58</v>
+      </c>
+      <c r="B357" s="0">
+        <v>44</v>
+      </c>
+      <c r="C357" s="0">
+        <v>55</v>
+      </c>
+      <c r="D357" s="0">
+        <v>41</v>
+      </c>
+      <c r="E357" s="0">
+        <v>43</v>
+      </c>
+      <c r="H357" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I357" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J357" s="0">
+        <v>0</v>
+      </c>
+      <c r="K357" s="0">
+        <v>58</v>
+      </c>
+      <c r="L357" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="0">
+        <v>52</v>
+      </c>
+      <c r="B358" s="0">
+        <v>38</v>
+      </c>
+      <c r="C358" s="0">
+        <v>54</v>
+      </c>
+      <c r="D358" s="0">
+        <v>35</v>
+      </c>
+      <c r="E358" s="0">
+        <v>30</v>
+      </c>
+      <c r="H358" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I358" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="J358" s="0">
+        <v>2</v>
+      </c>
+      <c r="K358" s="0">
+        <v>54</v>
+      </c>
+      <c r="L358" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="0">
+        <v>44</v>
+      </c>
+      <c r="B359" s="0">
+        <v>41</v>
+      </c>
+      <c r="C359" s="0">
+        <v>68</v>
+      </c>
+      <c r="D359" s="0">
+        <v>41</v>
+      </c>
+      <c r="E359" s="0">
+        <v>47</v>
+      </c>
+      <c r="H359" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I359" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J359" s="0">
+        <v>2</v>
+      </c>
+      <c r="K359" s="0">
+        <v>68</v>
+      </c>
+      <c r="L359" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="0">
+        <v>32</v>
+      </c>
+      <c r="B360" s="0">
+        <v>65</v>
+      </c>
+      <c r="C360" s="0">
+        <v>55</v>
+      </c>
+      <c r="D360" s="0">
+        <v>32</v>
+      </c>
+      <c r="E360" s="0">
+        <v>51</v>
+      </c>
+      <c r="H360" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I360" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J360" s="0">
+        <v>1</v>
+      </c>
+      <c r="K360" s="0">
+        <v>65</v>
+      </c>
+      <c r="L360" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="0">
+        <v>29</v>
+      </c>
+      <c r="B361" s="0">
+        <v>52</v>
+      </c>
+      <c r="C361" s="0">
+        <v>66</v>
+      </c>
+      <c r="D361" s="0">
+        <v>52</v>
+      </c>
+      <c r="E361" s="0">
+        <v>67</v>
+      </c>
+      <c r="H361" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I361" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J361" s="0">
+        <v>4</v>
+      </c>
+      <c r="K361" s="0">
+        <v>67</v>
+      </c>
+      <c r="L361" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="0">
+        <v>46</v>
+      </c>
+      <c r="B362" s="0">
+        <v>36</v>
+      </c>
+      <c r="C362" s="0">
+        <v>39</v>
+      </c>
+      <c r="D362" s="0">
+        <v>40</v>
+      </c>
+      <c r="E362" s="0">
+        <v>62</v>
+      </c>
+      <c r="H362" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I362" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J362" s="0">
+        <v>4</v>
+      </c>
+      <c r="K362" s="0">
+        <v>62</v>
+      </c>
+      <c r="L362" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="0">
+        <v>51</v>
+      </c>
+      <c r="B363" s="0">
+        <v>47</v>
+      </c>
+      <c r="C363" s="0">
+        <v>45</v>
+      </c>
+      <c r="D363" s="0">
+        <v>52</v>
+      </c>
+      <c r="E363" s="0">
+        <v>39</v>
+      </c>
+      <c r="H363" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I363" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J363" s="0">
+        <v>3</v>
+      </c>
+      <c r="K363" s="0">
+        <v>52</v>
+      </c>
+      <c r="L363" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="0">
+        <v>34</v>
+      </c>
+      <c r="B364" s="0">
+        <v>52</v>
+      </c>
+      <c r="C364" s="0">
+        <v>64</v>
+      </c>
+      <c r="D364" s="0">
+        <v>54</v>
+      </c>
+      <c r="E364" s="0">
+        <v>47</v>
+      </c>
+      <c r="H364" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I364" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J364" s="0">
+        <v>2</v>
+      </c>
+      <c r="K364" s="0">
+        <v>64</v>
+      </c>
+      <c r="L364" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="0">
+        <v>46</v>
+      </c>
+      <c r="B365" s="0">
+        <v>47</v>
+      </c>
+      <c r="C365" s="0">
+        <v>58</v>
+      </c>
+      <c r="D365" s="0">
+        <v>50</v>
+      </c>
+      <c r="E365" s="0">
+        <v>40</v>
+      </c>
+      <c r="H365" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I365" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J365" s="0">
+        <v>2</v>
+      </c>
+      <c r="K365" s="0">
+        <v>58</v>
+      </c>
+      <c r="L365" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="0">
+        <v>47</v>
+      </c>
+      <c r="B366" s="0">
+        <v>48</v>
+      </c>
+      <c r="C366" s="0">
+        <v>46</v>
+      </c>
+      <c r="D366" s="0">
+        <v>53</v>
+      </c>
+      <c r="E366" s="0">
+        <v>41</v>
+      </c>
+      <c r="H366" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I366" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J366" s="0">
+        <v>3</v>
+      </c>
+      <c r="K366" s="0">
+        <v>53</v>
+      </c>
+      <c r="L366" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" s="0">
+        <v>49</v>
+      </c>
+      <c r="B367" s="0">
+        <v>44</v>
+      </c>
+      <c r="C367" s="0">
+        <v>47</v>
+      </c>
+      <c r="D367" s="0">
+        <v>27</v>
+      </c>
+      <c r="E367" s="0">
+        <v>52</v>
+      </c>
+      <c r="H367" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I367" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J367" s="0">
+        <v>4</v>
+      </c>
+      <c r="K367" s="0">
+        <v>52</v>
+      </c>
+      <c r="L367" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="0">
+        <v>34</v>
+      </c>
+      <c r="B368" s="0">
+        <v>51</v>
+      </c>
+      <c r="C368" s="0">
+        <v>53</v>
+      </c>
+      <c r="D368" s="0">
+        <v>52</v>
+      </c>
+      <c r="E368" s="0">
+        <v>58</v>
+      </c>
+      <c r="H368" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I368" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="J368" s="0">
+        <v>4</v>
+      </c>
+      <c r="K368" s="0">
+        <v>58</v>
+      </c>
+      <c r="L368" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="0">
+        <v>49</v>
+      </c>
+      <c r="B369" s="0">
+        <v>38</v>
+      </c>
+      <c r="C369" s="0">
+        <v>71</v>
+      </c>
+      <c r="D369" s="0">
+        <v>35</v>
+      </c>
+      <c r="E369" s="0">
+        <v>52</v>
+      </c>
+      <c r="H369" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I369" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J369" s="0">
+        <v>2</v>
+      </c>
+      <c r="K369" s="0">
+        <v>71</v>
+      </c>
+      <c r="L369" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="0">
+        <v>48</v>
+      </c>
+      <c r="B370" s="0">
+        <v>50</v>
+      </c>
+      <c r="C370" s="0">
+        <v>52</v>
+      </c>
+      <c r="D370" s="0">
+        <v>59</v>
+      </c>
+      <c r="E370" s="0">
+        <v>35</v>
+      </c>
+      <c r="H370" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I370" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J370" s="0">
+        <v>3</v>
+      </c>
+      <c r="K370" s="0">
+        <v>59</v>
+      </c>
+      <c r="L370" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="0">
+        <v>44</v>
+      </c>
+      <c r="B371" s="0">
+        <v>35</v>
+      </c>
+      <c r="C371" s="0">
+        <v>64</v>
+      </c>
+      <c r="D371" s="0">
+        <v>41</v>
+      </c>
+      <c r="E371" s="0">
+        <v>65</v>
+      </c>
+      <c r="H371" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I371" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="J371" s="0">
+        <v>4</v>
+      </c>
+      <c r="K371" s="0">
+        <v>65</v>
+      </c>
+      <c r="L371" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="0">
+        <v>41</v>
+      </c>
+      <c r="B372" s="0">
+        <v>41</v>
+      </c>
+      <c r="C372" s="0">
+        <v>50</v>
+      </c>
+      <c r="D372" s="0">
+        <v>49</v>
+      </c>
+      <c r="E372" s="0">
+        <v>44</v>
+      </c>
+      <c r="H372" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I372" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J372" s="0">
+        <v>2</v>
+      </c>
+      <c r="K372" s="0">
+        <v>50</v>
+      </c>
+      <c r="L372" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="0">
+        <v>37</v>
+      </c>
+      <c r="B373" s="0">
+        <v>47</v>
+      </c>
+      <c r="C373" s="0">
+        <v>54</v>
+      </c>
+      <c r="D373" s="0">
+        <v>47</v>
+      </c>
+      <c r="E373" s="0">
+        <v>34</v>
+      </c>
+      <c r="H373" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I373" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J373" s="0">
+        <v>2</v>
+      </c>
+      <c r="K373" s="0">
+        <v>54</v>
+      </c>
+      <c r="L373" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="0">
+        <v>49</v>
+      </c>
+      <c r="B374" s="0">
+        <v>49</v>
+      </c>
+      <c r="C374" s="0">
+        <v>50</v>
+      </c>
+      <c r="D374" s="0">
+        <v>38</v>
+      </c>
+      <c r="E374" s="0">
+        <v>44</v>
+      </c>
+      <c r="H374" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I374" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J374" s="0">
+        <v>2</v>
+      </c>
+      <c r="K374" s="0">
+        <v>50</v>
+      </c>
+      <c r="L374" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="0">
+        <v>35</v>
+      </c>
+      <c r="B375" s="0">
+        <v>49</v>
+      </c>
+      <c r="C375" s="0">
+        <v>51</v>
+      </c>
+      <c r="D375" s="0">
+        <v>44</v>
+      </c>
+      <c r="E375" s="0">
+        <v>41</v>
+      </c>
+      <c r="H375" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I375" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J375" s="0">
+        <v>2</v>
+      </c>
+      <c r="K375" s="0">
+        <v>51</v>
+      </c>
+      <c r="L375" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="0">
+        <v>63</v>
+      </c>
+      <c r="B376" s="0">
+        <v>56</v>
+      </c>
+      <c r="C376" s="0">
+        <v>49</v>
+      </c>
+      <c r="D376" s="0">
+        <v>58</v>
+      </c>
+      <c r="E376" s="0">
+        <v>40</v>
+      </c>
+      <c r="H376" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I376" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J376" s="0">
+        <v>0</v>
+      </c>
+      <c r="K376" s="0">
+        <v>63</v>
+      </c>
+      <c r="L376" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="0">
+        <v>42</v>
+      </c>
+      <c r="B377" s="0">
+        <v>49</v>
+      </c>
+      <c r="C377" s="0">
+        <v>56</v>
+      </c>
+      <c r="D377" s="0">
+        <v>48</v>
+      </c>
+      <c r="E377" s="0">
+        <v>48</v>
+      </c>
+      <c r="H377" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I377" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J377" s="0">
+        <v>2</v>
+      </c>
+      <c r="K377" s="0">
+        <v>56</v>
+      </c>
+      <c r="L377" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="0">
+        <v>53</v>
+      </c>
+      <c r="B378" s="0">
+        <v>47</v>
+      </c>
+      <c r="C378" s="0">
+        <v>53</v>
+      </c>
+      <c r="D378" s="0">
+        <v>32</v>
+      </c>
+      <c r="E378" s="0">
+        <v>49</v>
+      </c>
+      <c r="H378" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I378" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J378" s="0">
+        <v>0</v>
+      </c>
+      <c r="K378" s="0">
+        <v>53</v>
+      </c>
+      <c r="L378" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="0">
+        <v>31</v>
+      </c>
+      <c r="B379" s="0">
+        <v>43</v>
+      </c>
+      <c r="C379" s="0">
+        <v>47</v>
+      </c>
+      <c r="D379" s="0">
+        <v>45</v>
+      </c>
+      <c r="E379" s="0">
+        <v>38</v>
+      </c>
+      <c r="H379" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I379" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J379" s="0">
+        <v>2</v>
+      </c>
+      <c r="K379" s="0">
+        <v>47</v>
+      </c>
+      <c r="L379" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="0">
+        <v>50</v>
+      </c>
+      <c r="B380" s="0">
+        <v>36</v>
+      </c>
+      <c r="C380" s="0">
+        <v>56</v>
+      </c>
+      <c r="D380" s="0">
+        <v>44</v>
+      </c>
+      <c r="E380" s="0">
+        <v>53</v>
+      </c>
+      <c r="H380" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I380" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J380" s="0">
+        <v>2</v>
+      </c>
+      <c r="K380" s="0">
+        <v>56</v>
+      </c>
+      <c r="L380" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="0">
+        <v>40</v>
+      </c>
+      <c r="B381" s="0">
+        <v>46</v>
+      </c>
+      <c r="C381" s="0">
+        <v>60</v>
+      </c>
+      <c r="D381" s="0">
+        <v>44</v>
+      </c>
+      <c r="E381" s="0">
+        <v>46</v>
+      </c>
+      <c r="H381" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="I381" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J381" s="0">
+        <v>2</v>
+      </c>
+      <c r="K381" s="0">
+        <v>60</v>
+      </c>
+      <c r="L381" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="0">
+        <v>43</v>
+      </c>
+      <c r="B382" s="0">
+        <v>36</v>
+      </c>
+      <c r="C382" s="0">
+        <v>48</v>
+      </c>
+      <c r="D382" s="0">
+        <v>44</v>
+      </c>
+      <c r="E382" s="0">
+        <v>54</v>
+      </c>
+      <c r="H382" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I382" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J382" s="0">
+        <v>4</v>
+      </c>
+      <c r="K382" s="0">
+        <v>54</v>
+      </c>
+      <c r="L382" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" s="0">
+        <v>44</v>
+      </c>
+      <c r="B383" s="0">
+        <v>43</v>
+      </c>
+      <c r="C383" s="0">
+        <v>56</v>
+      </c>
+      <c r="D383" s="0">
+        <v>58</v>
+      </c>
+      <c r="E383" s="0">
+        <v>49</v>
+      </c>
+      <c r="H383" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="I383" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J383" s="0">
+        <v>3</v>
+      </c>
+      <c r="K383" s="0">
+        <v>58</v>
+      </c>
+      <c r="L383" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" s="0">
+        <v>49</v>
+      </c>
+      <c r="B384" s="0">
+        <v>55</v>
+      </c>
+      <c r="C384" s="0">
+        <v>49</v>
+      </c>
+      <c r="D384" s="0">
+        <v>50</v>
+      </c>
+      <c r="E384" s="0">
+        <v>35</v>
+      </c>
+      <c r="H384" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I384" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J384" s="0">
+        <v>1</v>
+      </c>
+      <c r="K384" s="0">
+        <v>55</v>
+      </c>
+      <c r="L384" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="0">
+        <v>49</v>
+      </c>
+      <c r="B385" s="0">
+        <v>42</v>
+      </c>
+      <c r="C385" s="0">
+        <v>60</v>
+      </c>
+      <c r="D385" s="0">
+        <v>50</v>
+      </c>
+      <c r="E385" s="0">
+        <v>45</v>
+      </c>
+      <c r="H385" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I385" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J385" s="0">
+        <v>2</v>
+      </c>
+      <c r="K385" s="0">
+        <v>60</v>
+      </c>
+      <c r="L385" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" s="0">
+        <v>46</v>
+      </c>
+      <c r="B386" s="0">
+        <v>43</v>
+      </c>
+      <c r="C386" s="0">
+        <v>55</v>
+      </c>
+      <c r="D386" s="0">
+        <v>38</v>
+      </c>
+      <c r="E386" s="0">
+        <v>35</v>
+      </c>
+      <c r="H386" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I386" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J386" s="0">
+        <v>2</v>
+      </c>
+      <c r="K386" s="0">
+        <v>55</v>
+      </c>
+      <c r="L386" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="0">
+        <v>52</v>
+      </c>
+      <c r="B387" s="0">
+        <v>41</v>
+      </c>
+      <c r="C387" s="0">
+        <v>36</v>
+      </c>
+      <c r="D387" s="0">
+        <v>38</v>
+      </c>
+      <c r="E387" s="0">
+        <v>45</v>
+      </c>
+      <c r="H387" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I387" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J387" s="0">
+        <v>0</v>
+      </c>
+      <c r="K387" s="0">
+        <v>52</v>
+      </c>
+      <c r="L387" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="0">
+        <v>49</v>
+      </c>
+      <c r="B388" s="0">
+        <v>47</v>
+      </c>
+      <c r="C388" s="0">
+        <v>54</v>
+      </c>
+      <c r="D388" s="0">
+        <v>49</v>
+      </c>
+      <c r="E388" s="0">
+        <v>61</v>
+      </c>
+      <c r="H388" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I388" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J388" s="0">
+        <v>4</v>
+      </c>
+      <c r="K388" s="0">
+        <v>61</v>
+      </c>
+      <c r="L388" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="0">
+        <v>61</v>
+      </c>
+      <c r="B389" s="0">
+        <v>40</v>
+      </c>
+      <c r="C389" s="0">
+        <v>64</v>
+      </c>
+      <c r="D389" s="0">
+        <v>47</v>
+      </c>
+      <c r="E389" s="0">
+        <v>41</v>
+      </c>
+      <c r="H389" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I389" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J389" s="0">
+        <v>2</v>
+      </c>
+      <c r="K389" s="0">
+        <v>64</v>
+      </c>
+      <c r="L389" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="0">
+        <v>37</v>
+      </c>
+      <c r="B390" s="0">
+        <v>56</v>
+      </c>
+      <c r="C390" s="0">
+        <v>45</v>
+      </c>
+      <c r="D390" s="0">
+        <v>42</v>
+      </c>
+      <c r="E390" s="0">
+        <v>54</v>
+      </c>
+      <c r="H390" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I390" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J390" s="0">
+        <v>1</v>
+      </c>
+      <c r="K390" s="0">
+        <v>56</v>
+      </c>
+      <c r="L390" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="0">
+        <v>41</v>
+      </c>
+      <c r="B391" s="0">
+        <v>53</v>
+      </c>
+      <c r="C391" s="0">
+        <v>49</v>
+      </c>
+      <c r="D391" s="0">
+        <v>45</v>
+      </c>
+      <c r="E391" s="0">
+        <v>36</v>
+      </c>
+      <c r="H391" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I391" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J391" s="0">
+        <v>1</v>
+      </c>
+      <c r="K391" s="0">
+        <v>53</v>
+      </c>
+      <c r="L391" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="0">
+        <v>46</v>
+      </c>
+      <c r="B392" s="0">
+        <v>46</v>
+      </c>
+      <c r="C392" s="0">
+        <v>45</v>
+      </c>
+      <c r="D392" s="0">
+        <v>62</v>
+      </c>
+      <c r="E392" s="0">
+        <v>45</v>
+      </c>
+      <c r="H392" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I392" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J392" s="0">
+        <v>3</v>
+      </c>
+      <c r="K392" s="0">
+        <v>62</v>
+      </c>
+      <c r="L392" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" s="0">
+        <v>41</v>
+      </c>
+      <c r="B393" s="0">
+        <v>54</v>
+      </c>
+      <c r="C393" s="0">
+        <v>48</v>
+      </c>
+      <c r="D393" s="0">
+        <v>31</v>
+      </c>
+      <c r="E393" s="0">
+        <v>50</v>
+      </c>
+      <c r="H393" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I393" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J393" s="0">
+        <v>1</v>
+      </c>
+      <c r="K393" s="0">
+        <v>54</v>
+      </c>
+      <c r="L393" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="0">
+        <v>42</v>
+      </c>
+      <c r="B394" s="0">
+        <v>49</v>
+      </c>
+      <c r="C394" s="0">
+        <v>59</v>
+      </c>
+      <c r="D394" s="0">
+        <v>49</v>
+      </c>
+      <c r="E394" s="0">
+        <v>45</v>
+      </c>
+      <c r="H394" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I394" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J394" s="0">
+        <v>2</v>
+      </c>
+      <c r="K394" s="0">
+        <v>59</v>
+      </c>
+      <c r="L394" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="0">
+        <v>57</v>
+      </c>
+      <c r="B395" s="0">
+        <v>41</v>
+      </c>
+      <c r="C395" s="0">
+        <v>42</v>
+      </c>
+      <c r="D395" s="0">
+        <v>47</v>
+      </c>
+      <c r="E395" s="0">
+        <v>34</v>
+      </c>
+      <c r="H395" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I395" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J395" s="0">
+        <v>0</v>
+      </c>
+      <c r="K395" s="0">
+        <v>57</v>
+      </c>
+      <c r="L395" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="0">
+        <v>48</v>
+      </c>
+      <c r="B396" s="0">
+        <v>41</v>
+      </c>
+      <c r="C396" s="0">
+        <v>60</v>
+      </c>
+      <c r="D396" s="0">
+        <v>50</v>
+      </c>
+      <c r="E396" s="0">
+        <v>37</v>
+      </c>
+      <c r="H396" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="I396" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J396" s="0">
+        <v>2</v>
+      </c>
+      <c r="K396" s="0">
+        <v>60</v>
+      </c>
+      <c r="L396" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="0">
+        <v>39</v>
+      </c>
+      <c r="B397" s="0">
+        <v>35</v>
+      </c>
+      <c r="C397" s="0">
+        <v>59</v>
+      </c>
+      <c r="D397" s="0">
+        <v>54</v>
+      </c>
+      <c r="E397" s="0">
+        <v>57</v>
+      </c>
+      <c r="H397" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I397" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J397" s="0">
+        <v>2</v>
+      </c>
+      <c r="K397" s="0">
+        <v>59</v>
+      </c>
+      <c r="L397" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="0">
+        <v>45</v>
+      </c>
+      <c r="B398" s="0">
+        <v>53</v>
+      </c>
+      <c r="C398" s="0">
+        <v>49</v>
+      </c>
+      <c r="D398" s="0">
+        <v>46</v>
+      </c>
+      <c r="E398" s="0">
+        <v>47</v>
+      </c>
+      <c r="H398" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I398" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="J398" s="0">
+        <v>1</v>
+      </c>
+      <c r="K398" s="0">
+        <v>53</v>
+      </c>
+      <c r="L398" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="0">
+        <v>38</v>
+      </c>
+      <c r="B399" s="0">
+        <v>44</v>
+      </c>
+      <c r="C399" s="0">
+        <v>45</v>
+      </c>
+      <c r="D399" s="0">
+        <v>40</v>
+      </c>
+      <c r="E399" s="0">
+        <v>43</v>
+      </c>
+      <c r="H399" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="I399" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J399" s="0">
+        <v>2</v>
+      </c>
+      <c r="K399" s="0">
+        <v>45</v>
+      </c>
+      <c r="L399" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="0">
+        <v>42</v>
+      </c>
+      <c r="B400" s="0">
+        <v>44</v>
+      </c>
+      <c r="C400" s="0">
+        <v>58</v>
+      </c>
+      <c r="D400" s="0">
+        <v>59</v>
+      </c>
+      <c r="E400" s="0">
+        <v>43</v>
+      </c>
+      <c r="H400" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I400" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J400" s="0">
+        <v>3</v>
+      </c>
+      <c r="K400" s="0">
+        <v>59</v>
+      </c>
+      <c r="L400" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" s="0">
+        <v>35</v>
+      </c>
+      <c r="B401" s="0">
+        <v>43</v>
+      </c>
+      <c r="C401" s="0">
+        <v>56</v>
+      </c>
+      <c r="D401" s="0">
+        <v>39</v>
+      </c>
+      <c r="E401" s="0">
+        <v>52</v>
+      </c>
+      <c r="H401" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I401" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J401" s="0">
+        <v>2</v>
+      </c>
+      <c r="K401" s="0">
+        <v>56</v>
+      </c>
+      <c r="L401" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" s="0">
+        <v>38</v>
+      </c>
+      <c r="B402" s="0">
+        <v>44</v>
+      </c>
+      <c r="C402" s="0">
+        <v>48</v>
+      </c>
+      <c r="D402" s="0">
+        <v>52</v>
+      </c>
+      <c r="E402" s="0">
+        <v>41</v>
+      </c>
+      <c r="H402" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I402" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J402" s="0">
+        <v>3</v>
+      </c>
+      <c r="K402" s="0">
+        <v>52</v>
+      </c>
+      <c r="L402" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="0">
+        <v>44</v>
+      </c>
+      <c r="B403" s="0">
+        <v>49</v>
+      </c>
+      <c r="C403" s="0">
+        <v>60</v>
+      </c>
+      <c r="D403" s="0">
+        <v>40</v>
+      </c>
+      <c r="E403" s="0">
+        <v>46</v>
+      </c>
+      <c r="H403" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I403" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J403" s="0">
+        <v>2</v>
+      </c>
+      <c r="K403" s="0">
+        <v>60</v>
+      </c>
+      <c r="L403" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" s="0">
+        <v>54</v>
+      </c>
+      <c r="B404" s="0">
+        <v>39</v>
+      </c>
+      <c r="C404" s="0">
+        <v>62</v>
+      </c>
+      <c r="D404" s="0">
+        <v>52</v>
+      </c>
+      <c r="E404" s="0">
+        <v>50</v>
+      </c>
+      <c r="H404" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="I404" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J404" s="0">
+        <v>2</v>
+      </c>
+      <c r="K404" s="0">
+        <v>62</v>
+      </c>
+      <c r="L404" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="0">
+        <v>39</v>
+      </c>
+      <c r="B405" s="0">
+        <v>42</v>
+      </c>
+      <c r="C405" s="0">
+        <v>52</v>
+      </c>
+      <c r="D405" s="0">
+        <v>52</v>
+      </c>
+      <c r="E405" s="0">
+        <v>48</v>
+      </c>
+      <c r="H405" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I405" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J405" s="0">
+        <v>2</v>
+      </c>
+      <c r="K405" s="0">
+        <v>52</v>
+      </c>
+      <c r="L405" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" s="0">
+        <v>55</v>
+      </c>
+      <c r="B406" s="0">
+        <v>53</v>
+      </c>
+      <c r="C406" s="0">
+        <v>45</v>
+      </c>
+      <c r="D406" s="0">
+        <v>40</v>
+      </c>
+      <c r="E406" s="0">
+        <v>54</v>
+      </c>
+      <c r="H406" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I406" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J406" s="0">
+        <v>0</v>
+      </c>
+      <c r="K406" s="0">
+        <v>55</v>
+      </c>
+      <c r="L406" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" s="0">
+        <v>41</v>
+      </c>
+      <c r="B407" s="0">
+        <v>48</v>
+      </c>
+      <c r="C407" s="0">
+        <v>68</v>
+      </c>
+      <c r="D407" s="0">
+        <v>39</v>
+      </c>
+      <c r="E407" s="0">
+        <v>49</v>
+      </c>
+      <c r="H407" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I407" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J407" s="0">
+        <v>2</v>
+      </c>
+      <c r="K407" s="0">
+        <v>68</v>
+      </c>
+      <c r="L407" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="0">
+        <v>48</v>
+      </c>
+      <c r="B408" s="0">
+        <v>51</v>
+      </c>
+      <c r="C408" s="0">
+        <v>49</v>
+      </c>
+      <c r="D408" s="0">
+        <v>34</v>
+      </c>
+      <c r="E408" s="0">
+        <v>47</v>
+      </c>
+      <c r="H408" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I408" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J408" s="0">
+        <v>1</v>
+      </c>
+      <c r="K408" s="0">
+        <v>51</v>
+      </c>
+      <c r="L408" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="0">
+        <v>44</v>
+      </c>
+      <c r="B409" s="0">
+        <v>58</v>
+      </c>
+      <c r="C409" s="0">
+        <v>58</v>
+      </c>
+      <c r="D409" s="0">
+        <v>52</v>
+      </c>
+      <c r="E409" s="0">
+        <v>40</v>
+      </c>
+      <c r="H409" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I409" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J409" s="0">
+        <v>1</v>
+      </c>
+      <c r="K409" s="0">
+        <v>58</v>
+      </c>
+      <c r="L409" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="0">
+        <v>62</v>
+      </c>
+      <c r="B410" s="0">
+        <v>48</v>
+      </c>
+      <c r="C410" s="0">
+        <v>45</v>
+      </c>
+      <c r="D410" s="0">
+        <v>42</v>
+      </c>
+      <c r="E410" s="0">
+        <v>63</v>
+      </c>
+      <c r="H410" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I410" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J410" s="0">
+        <v>4</v>
+      </c>
+      <c r="K410" s="0">
+        <v>63</v>
+      </c>
+      <c r="L410" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="0">
+        <v>47</v>
+      </c>
+      <c r="B411" s="0">
+        <v>49</v>
+      </c>
+      <c r="C411" s="0">
+        <v>47</v>
+      </c>
+      <c r="D411" s="0">
+        <v>31</v>
+      </c>
+      <c r="E411" s="0">
+        <v>39</v>
+      </c>
+      <c r="H411" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I411" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J411" s="0">
+        <v>1</v>
+      </c>
+      <c r="K411" s="0">
+        <v>49</v>
+      </c>
+      <c r="L411" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" s="0">
+        <v>72</v>
+      </c>
+      <c r="B412" s="0">
+        <v>33</v>
+      </c>
+      <c r="C412" s="0">
+        <v>51</v>
+      </c>
+      <c r="D412" s="0">
+        <v>54</v>
+      </c>
+      <c r="E412" s="0">
+        <v>42</v>
+      </c>
+      <c r="H412" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I412" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J412" s="0">
+        <v>0</v>
+      </c>
+      <c r="K412" s="0">
+        <v>72</v>
+      </c>
+      <c r="L412" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" s="0">
+        <v>54</v>
+      </c>
+      <c r="B413" s="0">
+        <v>52</v>
+      </c>
+      <c r="C413" s="0">
+        <v>51</v>
+      </c>
+      <c r="D413" s="0">
+        <v>36</v>
+      </c>
+      <c r="E413" s="0">
+        <v>47</v>
+      </c>
+      <c r="H413" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I413" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J413" s="0">
+        <v>0</v>
+      </c>
+      <c r="K413" s="0">
+        <v>54</v>
+      </c>
+      <c r="L413" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" s="0">
+        <v>52</v>
+      </c>
+      <c r="B414" s="0">
+        <v>57</v>
+      </c>
+      <c r="C414" s="0">
+        <v>70</v>
+      </c>
+      <c r="D414" s="0">
+        <v>51</v>
+      </c>
+      <c r="E414" s="0">
+        <v>18</v>
+      </c>
+      <c r="H414" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I414" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J414" s="0">
+        <v>2</v>
+      </c>
+      <c r="K414" s="0">
+        <v>70</v>
+      </c>
+      <c r="L414" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="0">
+        <v>41</v>
+      </c>
+      <c r="B415" s="0">
+        <v>43</v>
+      </c>
+      <c r="C415" s="0">
+        <v>46</v>
+      </c>
+      <c r="D415" s="0">
+        <v>51</v>
+      </c>
+      <c r="E415" s="0">
+        <v>57</v>
+      </c>
+      <c r="H415" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I415" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J415" s="0">
+        <v>4</v>
+      </c>
+      <c r="K415" s="0">
+        <v>57</v>
+      </c>
+      <c r="L415" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" s="0">
+        <v>47</v>
+      </c>
+      <c r="B416" s="0">
+        <v>48</v>
+      </c>
+      <c r="C416" s="0">
+        <v>43</v>
+      </c>
+      <c r="D416" s="0">
+        <v>42</v>
+      </c>
+      <c r="E416" s="0">
+        <v>42</v>
+      </c>
+      <c r="H416" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I416" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J416" s="0">
+        <v>1</v>
+      </c>
+      <c r="K416" s="0">
+        <v>48</v>
+      </c>
+      <c r="L416" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" s="0">
+        <v>52</v>
+      </c>
+      <c r="B417" s="0">
+        <v>40</v>
+      </c>
+      <c r="C417" s="0">
+        <v>38</v>
+      </c>
+      <c r="D417" s="0">
+        <v>43</v>
+      </c>
+      <c r="E417" s="0">
+        <v>47</v>
+      </c>
+      <c r="H417" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I417" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J417" s="0">
+        <v>0</v>
+      </c>
+      <c r="K417" s="0">
+        <v>52</v>
+      </c>
+      <c r="L417" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" s="0">
+        <v>56</v>
+      </c>
+      <c r="B418" s="0">
+        <v>36</v>
+      </c>
+      <c r="C418" s="0">
+        <v>47</v>
+      </c>
+      <c r="D418" s="0">
+        <v>58</v>
+      </c>
+      <c r="E418" s="0">
+        <v>40</v>
+      </c>
+      <c r="H418" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I418" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J418" s="0">
+        <v>3</v>
+      </c>
+      <c r="K418" s="0">
+        <v>58</v>
+      </c>
+      <c r="L418" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" s="0">
+        <v>36</v>
+      </c>
+      <c r="B419" s="0">
+        <v>54</v>
+      </c>
+      <c r="C419" s="0">
+        <v>51</v>
+      </c>
+      <c r="D419" s="0">
+        <v>33</v>
+      </c>
+      <c r="E419" s="0">
+        <v>53</v>
+      </c>
+      <c r="H419" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I419" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J419" s="0">
+        <v>1</v>
+      </c>
+      <c r="K419" s="0">
+        <v>54</v>
+      </c>
+      <c r="L419" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" s="0">
+        <v>35</v>
+      </c>
+      <c r="B420" s="0">
+        <v>39</v>
+      </c>
+      <c r="C420" s="0">
+        <v>60</v>
+      </c>
+      <c r="D420" s="0">
+        <v>50</v>
+      </c>
+      <c r="E420" s="0">
+        <v>40</v>
+      </c>
+      <c r="H420" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I420" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J420" s="0">
+        <v>2</v>
+      </c>
+      <c r="K420" s="0">
+        <v>60</v>
+      </c>
+      <c r="L420" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" s="0">
+        <v>39</v>
+      </c>
+      <c r="B421" s="0">
+        <v>47</v>
+      </c>
+      <c r="C421" s="0">
+        <v>52</v>
+      </c>
+      <c r="D421" s="0">
+        <v>49</v>
+      </c>
+      <c r="E421" s="0">
+        <v>54</v>
+      </c>
+      <c r="H421" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I421" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J421" s="0">
+        <v>4</v>
+      </c>
+      <c r="K421" s="0">
+        <v>54</v>
+      </c>
+      <c r="L421" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" s="0">
+        <v>59</v>
+      </c>
+      <c r="B422" s="0">
+        <v>29</v>
+      </c>
+      <c r="C422" s="0">
+        <v>45</v>
+      </c>
+      <c r="D422" s="0">
+        <v>55</v>
+      </c>
+      <c r="E422" s="0">
+        <v>37</v>
+      </c>
+      <c r="H422" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I422" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J422" s="0">
+        <v>0</v>
+      </c>
+      <c r="K422" s="0">
+        <v>59</v>
+      </c>
+      <c r="L422" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" s="0">
+        <v>45</v>
+      </c>
+      <c r="B423" s="0">
+        <v>36</v>
+      </c>
+      <c r="C423" s="0">
+        <v>58</v>
+      </c>
+      <c r="D423" s="0">
+        <v>39</v>
+      </c>
+      <c r="E423" s="0">
+        <v>51</v>
+      </c>
+      <c r="H423" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I423" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J423" s="0">
+        <v>2</v>
+      </c>
+      <c r="K423" s="0">
+        <v>58</v>
+      </c>
+      <c r="L423" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" s="0">
+        <v>49</v>
+      </c>
+      <c r="B424" s="0">
+        <v>26</v>
+      </c>
+      <c r="C424" s="0">
+        <v>68</v>
+      </c>
+      <c r="D424" s="0">
+        <v>41</v>
+      </c>
+      <c r="E424" s="0">
+        <v>53</v>
+      </c>
+      <c r="H424" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I424" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J424" s="0">
+        <v>2</v>
+      </c>
+      <c r="K424" s="0">
+        <v>68</v>
+      </c>
+      <c r="L424" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" s="0">
+        <v>60</v>
+      </c>
+      <c r="B425" s="0">
+        <v>39</v>
+      </c>
+      <c r="C425" s="0">
+        <v>55</v>
+      </c>
+      <c r="D425" s="0">
+        <v>41</v>
+      </c>
+      <c r="E425" s="0">
+        <v>63</v>
+      </c>
+      <c r="H425" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I425" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J425" s="0">
+        <v>4</v>
+      </c>
+      <c r="K425" s="0">
+        <v>63</v>
+      </c>
+      <c r="L425" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" s="0">
+        <v>44</v>
+      </c>
+      <c r="B426" s="0">
+        <v>43</v>
+      </c>
+      <c r="C426" s="0">
+        <v>49</v>
+      </c>
+      <c r="D426" s="0">
+        <v>52</v>
+      </c>
+      <c r="E426" s="0">
+        <v>45</v>
+      </c>
+      <c r="H426" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I426" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J426" s="0">
+        <v>3</v>
+      </c>
+      <c r="K426" s="0">
+        <v>52</v>
+      </c>
+      <c r="L426" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" s="0">
+        <v>58</v>
+      </c>
+      <c r="B427" s="0">
+        <v>42</v>
+      </c>
+      <c r="C427" s="0">
+        <v>51</v>
+      </c>
+      <c r="D427" s="0">
+        <v>51</v>
+      </c>
+      <c r="E427" s="0">
+        <v>42</v>
+      </c>
+      <c r="H427" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I427" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J427" s="0">
+        <v>0</v>
+      </c>
+      <c r="K427" s="0">
+        <v>58</v>
+      </c>
+      <c r="L427" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" s="0">
+        <v>55</v>
+      </c>
+      <c r="B428" s="0">
+        <v>52</v>
+      </c>
+      <c r="C428" s="0">
+        <v>36</v>
+      </c>
+      <c r="D428" s="0">
+        <v>63</v>
+      </c>
+      <c r="E428" s="0">
+        <v>39</v>
+      </c>
+      <c r="H428" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I428" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J428" s="0">
+        <v>3</v>
+      </c>
+      <c r="K428" s="0">
+        <v>63</v>
+      </c>
+      <c r="L428" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" s="0">
+        <v>46</v>
+      </c>
+      <c r="B429" s="0">
+        <v>36</v>
+      </c>
+      <c r="C429" s="0">
+        <v>57</v>
+      </c>
+      <c r="D429" s="0">
+        <v>53</v>
+      </c>
+      <c r="E429" s="0">
+        <v>53</v>
+      </c>
+      <c r="H429" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I429" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J429" s="0">
+        <v>2</v>
+      </c>
+      <c r="K429" s="0">
+        <v>57</v>
+      </c>
+      <c r="L429" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" s="0">
+        <v>51</v>
+      </c>
+      <c r="B430" s="0">
+        <v>43</v>
+      </c>
+      <c r="C430" s="0">
+        <v>57</v>
+      </c>
+      <c r="D430" s="0">
+        <v>27</v>
+      </c>
+      <c r="E430" s="0">
+        <v>53</v>
+      </c>
+      <c r="H430" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I430" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J430" s="0">
+        <v>2</v>
+      </c>
+      <c r="K430" s="0">
+        <v>57</v>
+      </c>
+      <c r="L430" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" s="0">
+        <v>52</v>
+      </c>
+      <c r="B431" s="0">
+        <v>46</v>
+      </c>
+      <c r="C431" s="0">
+        <v>71</v>
+      </c>
+      <c r="D431" s="0">
+        <v>38</v>
+      </c>
+      <c r="E431" s="0">
+        <v>48</v>
+      </c>
+      <c r="H431" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I431" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J431" s="0">
+        <v>2</v>
+      </c>
+      <c r="K431" s="0">
+        <v>71</v>
+      </c>
+      <c r="L431" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" s="0">
+        <v>49</v>
+      </c>
+      <c r="B432" s="0">
+        <v>39</v>
+      </c>
+      <c r="C432" s="0">
+        <v>66</v>
+      </c>
+      <c r="D432" s="0">
+        <v>48</v>
+      </c>
+      <c r="E432" s="0">
+        <v>51</v>
+      </c>
+      <c r="H432" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I432" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J432" s="0">
+        <v>2</v>
+      </c>
+      <c r="K432" s="0">
+        <v>66</v>
+      </c>
+      <c r="L432" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" s="0">
+        <v>38</v>
+      </c>
+      <c r="B433" s="0">
+        <v>27</v>
+      </c>
+      <c r="C433" s="0">
+        <v>64</v>
+      </c>
+      <c r="D433" s="0">
+        <v>56</v>
+      </c>
+      <c r="E433" s="0">
+        <v>53</v>
+      </c>
+      <c r="H433" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I433" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J433" s="0">
+        <v>2</v>
+      </c>
+      <c r="K433" s="0">
+        <v>64</v>
+      </c>
+      <c r="L433" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" s="0">
+        <v>55</v>
+      </c>
+      <c r="B434" s="0">
+        <v>33</v>
+      </c>
+      <c r="C434" s="0">
+        <v>46</v>
+      </c>
+      <c r="D434" s="0">
+        <v>50</v>
+      </c>
+      <c r="E434" s="0">
+        <v>38</v>
+      </c>
+      <c r="H434" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I434" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J434" s="0">
+        <v>0</v>
+      </c>
+      <c r="K434" s="0">
+        <v>55</v>
+      </c>
+      <c r="L434" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" s="0">
+        <v>38</v>
+      </c>
+      <c r="B435" s="0">
+        <v>58</v>
+      </c>
+      <c r="C435" s="0">
+        <v>52</v>
+      </c>
+      <c r="D435" s="0">
+        <v>37</v>
+      </c>
+      <c r="E435" s="0">
+        <v>46</v>
+      </c>
+      <c r="H435" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I435" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J435" s="0">
+        <v>1</v>
+      </c>
+      <c r="K435" s="0">
+        <v>58</v>
+      </c>
+      <c r="L435" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" s="0">
+        <v>40</v>
+      </c>
+      <c r="B436" s="0">
+        <v>24</v>
+      </c>
+      <c r="C436" s="0">
+        <v>76</v>
+      </c>
+      <c r="D436" s="0">
+        <v>45</v>
+      </c>
+      <c r="E436" s="0">
+        <v>43</v>
+      </c>
+      <c r="H436" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I436" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J436" s="0">
+        <v>2</v>
+      </c>
+      <c r="K436" s="0">
+        <v>76</v>
+      </c>
+      <c r="L436" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" s="0">
+        <v>56</v>
+      </c>
+      <c r="B437" s="0">
+        <v>45</v>
+      </c>
+      <c r="C437" s="0">
+        <v>51</v>
+      </c>
+      <c r="D437" s="0">
+        <v>49</v>
+      </c>
+      <c r="E437" s="0">
+        <v>38</v>
+      </c>
+      <c r="H437" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I437" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J437" s="0">
+        <v>0</v>
+      </c>
+      <c r="K437" s="0">
+        <v>56</v>
+      </c>
+      <c r="L437" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" s="0">
+        <v>47</v>
+      </c>
+      <c r="B438" s="0">
+        <v>42</v>
+      </c>
+      <c r="C438" s="0">
+        <v>44</v>
+      </c>
+      <c r="D438" s="0">
+        <v>45</v>
+      </c>
+      <c r="E438" s="0">
+        <v>41</v>
+      </c>
+      <c r="H438" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I438" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J438" s="0">
+        <v>0</v>
+      </c>
+      <c r="K438" s="0">
+        <v>47</v>
+      </c>
+      <c r="L438" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="0">
+        <v>39</v>
+      </c>
+      <c r="B439" s="0">
+        <v>33</v>
+      </c>
+      <c r="C439" s="0">
+        <v>62</v>
+      </c>
+      <c r="D439" s="0">
+        <v>46</v>
+      </c>
+      <c r="E439" s="0">
+        <v>48</v>
+      </c>
+      <c r="H439" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I439" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J439" s="0">
+        <v>2</v>
+      </c>
+      <c r="K439" s="0">
+        <v>62</v>
+      </c>
+      <c r="L439" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" s="0">
+        <v>51</v>
+      </c>
+      <c r="B440" s="0">
+        <v>56</v>
+      </c>
+      <c r="C440" s="0">
+        <v>55</v>
+      </c>
+      <c r="D440" s="0">
+        <v>46</v>
+      </c>
+      <c r="E440" s="0">
+        <v>48</v>
+      </c>
+      <c r="H440" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I440" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J440" s="0">
+        <v>1</v>
+      </c>
+      <c r="K440" s="0">
+        <v>56</v>
+      </c>
+      <c r="L440" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" s="0">
+        <v>56</v>
+      </c>
+      <c r="B441" s="0">
+        <v>50</v>
+      </c>
+      <c r="C441" s="0">
+        <v>43</v>
+      </c>
+      <c r="D441" s="0">
+        <v>49</v>
+      </c>
+      <c r="E441" s="0">
+        <v>53</v>
+      </c>
+      <c r="H441" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I441" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="J441" s="0">
+        <v>0</v>
+      </c>
+      <c r="K441" s="0">
+        <v>56</v>
+      </c>
+      <c r="L441" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" s="0">
+        <v>45</v>
+      </c>
+      <c r="B442" s="0">
+        <v>43</v>
+      </c>
+      <c r="C442" s="0">
+        <v>61</v>
+      </c>
+      <c r="D442" s="0">
+        <v>47</v>
+      </c>
+      <c r="E442" s="0">
+        <v>48</v>
+      </c>
+      <c r="H442" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I442" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J442" s="0">
+        <v>2</v>
+      </c>
+      <c r="K442" s="0">
+        <v>61</v>
+      </c>
+      <c r="L442" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" s="0">
+        <v>22</v>
+      </c>
+      <c r="B443" s="0">
+        <v>61</v>
+      </c>
+      <c r="C443" s="0">
+        <v>61</v>
+      </c>
+      <c r="D443" s="0">
+        <v>34</v>
+      </c>
+      <c r="E443" s="0">
+        <v>65</v>
+      </c>
+      <c r="H443" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I443" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J443" s="0">
+        <v>4</v>
+      </c>
+      <c r="K443" s="0">
+        <v>65</v>
+      </c>
+      <c r="L443" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" s="0">
+        <v>52</v>
+      </c>
+      <c r="B444" s="0">
+        <v>37</v>
+      </c>
+      <c r="C444" s="0">
+        <v>59</v>
+      </c>
+      <c r="D444" s="0">
+        <v>50</v>
+      </c>
+      <c r="E444" s="0">
+        <v>46</v>
+      </c>
+      <c r="H444" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I444" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J444" s="0">
+        <v>2</v>
+      </c>
+      <c r="K444" s="0">
+        <v>59</v>
+      </c>
+      <c r="L444" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" s="0">
+        <v>30</v>
+      </c>
+      <c r="B445" s="0">
+        <v>41</v>
+      </c>
+      <c r="C445" s="0">
+        <v>51</v>
+      </c>
+      <c r="D445" s="0">
+        <v>46</v>
+      </c>
+      <c r="E445" s="0">
+        <v>50</v>
+      </c>
+      <c r="H445" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I445" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J445" s="0">
+        <v>2</v>
+      </c>
+      <c r="K445" s="0">
+        <v>51</v>
+      </c>
+      <c r="L445" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" s="0">
+        <v>45</v>
+      </c>
+      <c r="B446" s="0">
+        <v>39</v>
+      </c>
+      <c r="C446" s="0">
+        <v>78</v>
+      </c>
+      <c r="D446" s="0">
+        <v>42</v>
+      </c>
+      <c r="E446" s="0">
+        <v>52</v>
+      </c>
+      <c r="H446" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I446" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J446" s="0">
+        <v>2</v>
+      </c>
+      <c r="K446" s="0">
+        <v>78</v>
+      </c>
+      <c r="L446" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" s="0">
+        <v>42</v>
+      </c>
+      <c r="B447" s="0">
+        <v>48</v>
+      </c>
+      <c r="C447" s="0">
+        <v>52</v>
+      </c>
+      <c r="D447" s="0">
+        <v>51</v>
+      </c>
+      <c r="E447" s="0">
+        <v>39</v>
+      </c>
+      <c r="H447" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I447" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="J447" s="0">
+        <v>2</v>
+      </c>
+      <c r="K447" s="0">
+        <v>52</v>
+      </c>
+      <c r="L447" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" s="0">
+        <v>49</v>
+      </c>
+      <c r="B448" s="0">
+        <v>34</v>
+      </c>
+      <c r="C448" s="0">
+        <v>62</v>
+      </c>
+      <c r="D448" s="0">
+        <v>41</v>
+      </c>
+      <c r="E448" s="0">
+        <v>50</v>
+      </c>
+      <c r="H448" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I448" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J448" s="0">
+        <v>2</v>
+      </c>
+      <c r="K448" s="0">
+        <v>62</v>
+      </c>
+      <c r="L448" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" s="0">
+        <v>70</v>
+      </c>
+      <c r="B449" s="0">
+        <v>48</v>
+      </c>
+      <c r="C449" s="0">
+        <v>65</v>
+      </c>
+      <c r="D449" s="0">
+        <v>37</v>
+      </c>
+      <c r="E449" s="0">
+        <v>46</v>
+      </c>
+      <c r="H449" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I449" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J449" s="0">
+        <v>0</v>
+      </c>
+      <c r="K449" s="0">
+        <v>70</v>
+      </c>
+      <c r="L449" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" s="0">
+        <v>55</v>
+      </c>
+      <c r="B450" s="0">
+        <v>43</v>
+      </c>
+      <c r="C450" s="0">
+        <v>50</v>
+      </c>
+      <c r="D450" s="0">
+        <v>43</v>
+      </c>
+      <c r="E450" s="0">
+        <v>67</v>
+      </c>
+      <c r="H450" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I450" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J450" s="0">
+        <v>4</v>
+      </c>
+      <c r="K450" s="0">
+        <v>67</v>
+      </c>
+      <c r="L450" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" s="0">
+        <v>57</v>
+      </c>
+      <c r="B451" s="0">
+        <v>41</v>
+      </c>
+      <c r="C451" s="0">
+        <v>51</v>
+      </c>
+      <c r="D451" s="0">
+        <v>39</v>
+      </c>
+      <c r="E451" s="0">
+        <v>39</v>
+      </c>
+      <c r="H451" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I451" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J451" s="0">
+        <v>0</v>
+      </c>
+      <c r="K451" s="0">
+        <v>57</v>
+      </c>
+      <c r="L451" s="0">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>